<commit_message>
working needs mayor refactors
</commit_message>
<xml_diff>
--- a/Leerplanillacupos/output_Insciptos ID y AN al 09 08 24.xlsx
+++ b/Leerplanillacupos/output_Insciptos ID y AN al 09 08 24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,11 @@
           <t>Cupos</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -532,6 +537,11 @@
           <t>28</t>
         </is>
       </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -580,6 +590,11 @@
           <t>33</t>
         </is>
       </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -628,6 +643,11 @@
           <t>33</t>
         </is>
       </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -676,6 +696,11 @@
           <t>30</t>
         </is>
       </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -724,6 +749,11 @@
           <t>30</t>
         </is>
       </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -772,6 +802,11 @@
           <t>30</t>
         </is>
       </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -820,6 +855,11 @@
           <t>30</t>
         </is>
       </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -868,6 +908,11 @@
           <t>30</t>
         </is>
       </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -916,6 +961,11 @@
           <t>30</t>
         </is>
       </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -964,6 +1014,11 @@
           <t>30</t>
         </is>
       </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1012,6 +1067,11 @@
           <t>30</t>
         </is>
       </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1060,6 +1120,11 @@
           <t>30</t>
         </is>
       </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1108,6 +1173,11 @@
           <t>42</t>
         </is>
       </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1156,6 +1226,11 @@
           <t>30</t>
         </is>
       </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1204,6 +1279,11 @@
           <t>30</t>
         </is>
       </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1252,6 +1332,11 @@
           <t>30</t>
         </is>
       </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1300,6 +1385,11 @@
           <t>32</t>
         </is>
       </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1348,6 +1438,11 @@
           <t>30</t>
         </is>
       </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1396,6 +1491,11 @@
           <t>30</t>
         </is>
       </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1444,6 +1544,11 @@
           <t>30</t>
         </is>
       </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1492,6 +1597,11 @@
           <t>30</t>
         </is>
       </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1538,6 +1648,11 @@
       <c r="J23" t="inlineStr">
         <is>
           <t>31</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
refactored to delete all code to handle unnamed columns
</commit_message>
<xml_diff>
--- a/Leerplanillacupos/output_Insciptos ID y AN al 09 08 24.xlsx
+++ b/Leerplanillacupos/output_Insciptos ID y AN al 09 08 24.xlsx
@@ -539,7 +539,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -592,7 +592,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -804,7 +804,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -857,7 +857,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -910,7 +910,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -963,7 +963,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -1122,7 +1122,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -1440,7 +1440,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -1493,7 +1493,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -1599,7 +1599,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>
@@ -1652,7 +1652,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>09 08 24</t>
+          <t>09/08/24</t>
         </is>
       </c>
     </row>

</xml_diff>